<commit_message>
Added TODO list and added more code
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E78EA4C-CE7B-4F29-9759-C9E304EA6813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GopherCAN Message" sheetId="2" r:id="rId1"/>
+    <sheet name="Moduals" sheetId="1" r:id="rId2"/>
+    <sheet name="Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="Commands" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +27,134 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>ID (Decimal)</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>The GM internal name of the modual refrecenced</t>
+  </si>
+  <si>
+    <t>The ID of this modual in decimal format. Max = 64 (6 bits)</t>
+  </si>
+  <si>
+    <t>ECM</t>
+  </si>
+  <si>
+    <t>EDL</t>
+  </si>
+  <si>
+    <t>PDM</t>
+  </si>
+  <si>
+    <t>TCM</t>
+  </si>
+  <si>
+    <t>ACM</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Destination Node</t>
+  </si>
+  <si>
+    <t>Source Node</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>High Priority</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>No Error</t>
+  </si>
+  <si>
+    <t>Parameter Name</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>DLC (Decimal)</t>
+  </si>
+  <si>
+    <t>The Gopher Motersports internal name of the modual refrecenced</t>
+  </si>
+  <si>
+    <t>The ID of this parameter in decimal format. Max = 32768 (15 bits)</t>
+  </si>
+  <si>
+    <t>Final data type (u8, float, ect). Each data type will have a specific ID</t>
+  </si>
+  <si>
+    <t>The number of bytes this message needs for this parameter. This is directly related to the data type</t>
+  </si>
+  <si>
+    <t>Request Value</t>
+  </si>
+  <si>
+    <t>u16 (15 bits used)</t>
+  </si>
+  <si>
+    <t>Custom Command</t>
+  </si>
+  <si>
+    <t>u16</t>
+  </si>
+  <si>
+    <t>FAN_CURRENT</t>
+  </si>
+  <si>
+    <t>Command Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>INC_VARIABLE</t>
+  </si>
+  <si>
+    <t>TURN_FAN_OFF</t>
+  </si>
+  <si>
+    <t>CUST_COMMAND_2</t>
+  </si>
+  <si>
+    <t>2x u8</t>
+  </si>
+  <si>
+    <t>8 bits for command ID, 8 bits for function parameter</t>
+  </si>
+  <si>
+    <t>This will be used for requesting data from another module</t>
+  </si>
+  <si>
+    <t>Max 255 (U8)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +162,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE06666"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +240,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +555,573 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A1" s="3">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6">
+        <v>0</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:AB2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="15.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="102" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="17.07421875" customWidth="1"/>
+    <col min="2" max="2" width="25.765625" customWidth="1"/>
+    <col min="3" max="3" width="19.84375" customWidth="1"/>
+    <col min="4" max="4" width="14.61328125" customWidth="1"/>
+    <col min="5" max="5" width="23.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="91.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB27F71-B657-4A76-B4D2-CB1DD8552EDE}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="23.61328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="37.299999999999997" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added complete examples to the GpherCAN spreadsheet
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calja\GitHub Files\Gopher Motorsports\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E78EA4C-CE7B-4F29-9759-C9E304EA6813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AD2FB9-DFC6-4CBB-BBB5-4C82B9F3D392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GopherCAN Message" sheetId="2" r:id="rId1"/>
-    <sheet name="Moduals" sheetId="1" r:id="rId2"/>
-    <sheet name="Parameters" sheetId="3" r:id="rId3"/>
-    <sheet name="Commands" sheetId="4" r:id="rId4"/>
+    <sheet name="Moduals" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameters" sheetId="3" r:id="rId2"/>
+    <sheet name="Commands" sheetId="4" r:id="rId3"/>
+    <sheet name="ID Example" sheetId="2" r:id="rId4"/>
+    <sheet name="Full Message Examples" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
   <si>
     <t>Module Name</t>
   </si>
@@ -111,15 +112,9 @@
     <t>Request Value</t>
   </si>
   <si>
-    <t>u16 (15 bits used)</t>
-  </si>
-  <si>
     <t>Custom Command</t>
   </si>
   <si>
-    <t>u16</t>
-  </si>
-  <si>
     <t>FAN_CURRENT</t>
   </si>
   <si>
@@ -138,9 +133,6 @@
     <t>CUST_COMMAND_2</t>
   </si>
   <si>
-    <t>2x u8</t>
-  </si>
-  <si>
     <t>8 bits for command ID, 8 bits for function parameter</t>
   </si>
   <si>
@@ -148,6 +140,141 @@
   </si>
   <si>
     <t>Max 255 (U8)</t>
+  </si>
+  <si>
+    <t>COMMAND</t>
+  </si>
+  <si>
+    <t>REQ_PARAM</t>
+  </si>
+  <si>
+    <t>U16</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>Request Example</t>
+  </si>
+  <si>
+    <t>[1, 6]</t>
+  </si>
+  <si>
+    <t>[7, 12]</t>
+  </si>
+  <si>
+    <t>[14, 28]</t>
+  </si>
+  <si>
+    <t>Data Exmple</t>
+  </si>
+  <si>
+    <t>Low Priority</t>
+  </si>
+  <si>
+    <t>DLC</t>
+  </si>
+  <si>
+    <t>[0, 3]</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>byte 0</t>
+  </si>
+  <si>
+    <t>byte 1</t>
+  </si>
+  <si>
+    <t>byte 2</t>
+  </si>
+  <si>
+    <t>byte 3</t>
+  </si>
+  <si>
+    <t>byte 4</t>
+  </si>
+  <si>
+    <t>byte 5</t>
+  </si>
+  <si>
+    <t>byte 6</t>
+  </si>
+  <si>
+    <t>byte 7</t>
+  </si>
+  <si>
+    <t>[0, 7]</t>
+  </si>
+  <si>
+    <t>[8, 15]</t>
+  </si>
+  <si>
+    <t>[16, 23]</t>
+  </si>
+  <si>
+    <t>[24, 31]</t>
+  </si>
+  <si>
+    <t>[32, 39]</t>
+  </si>
+  <si>
+    <t>Number of Bytes</t>
+  </si>
+  <si>
+    <t>[40, 47]</t>
+  </si>
+  <si>
+    <t>[48, 55]</t>
+  </si>
+  <si>
+    <t>[56, 63]</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0x0</t>
+  </si>
+  <si>
+    <t>0x2</t>
+  </si>
+  <si>
+    <t>0x4</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>0xE8</t>
+  </si>
+  <si>
+    <t>Value = 1000</t>
+  </si>
+  <si>
+    <t>Req_Param</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>CAN Command Example</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>TURN_OFF_FAN</t>
+  </si>
+  <si>
+    <t>Parameter 0</t>
+  </si>
+  <si>
+    <t>0x1</t>
   </si>
 </sst>
 </file>
@@ -184,7 +311,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +354,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -240,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -275,6 +438,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,16 +748,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
-  <dimension ref="A1:AC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="91.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB27F71-B657-4A76-B4D2-CB1DD8552EDE}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
+  <dimension ref="A1:AC10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -653,7 +1107,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -673,10 +1127,12 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -690,11 +1146,9 @@
       <c r="Z2" s="12"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
-      <c r="AC2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="AC2" s="12"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -725,7 +1179,7 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -805,16 +1259,16 @@
         <v>0</v>
       </c>
       <c r="AA4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="6">
         <v>1</v>
       </c>
-      <c r="AB4" s="6">
-        <v>0</v>
-      </c>
       <c r="AC4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -834,7 +1288,9 @@
       <c r="M5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -848,279 +1304,351 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1" t="s">
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AC5" s="1" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="10" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:M2"/>
-    <mergeCell ref="N2:AB2"/>
+    <mergeCell ref="O2:AC2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="15.15234375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="102" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
-  <dimension ref="A1:E6"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8270471-FF49-4B7E-9E01-25107B918C4F}">
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="17.07421875" customWidth="1"/>
-    <col min="2" max="2" width="25.765625" customWidth="1"/>
-    <col min="3" max="3" width="19.84375" customWidth="1"/>
-    <col min="4" max="4" width="14.61328125" customWidth="1"/>
-    <col min="5" max="5" width="23.53515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="91.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="20">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="20">
+        <v>13</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O10" t="s">
+        <v>67</v>
+      </c>
+      <c r="P10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB27F71-B657-4A76-B4D2-CB1DD8552EDE}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="23.61328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="37.299999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.3" customHeight="1" x14ac:dyDescent="0.4"/>
+      <c r="I15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FEAT] added lots of stuff, including bitwise example messages in the XLSX file
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calja\GitHub Files\Gopher Motorsports\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AD2FB9-DFC6-4CBB-BBB5-4C82B9F3D392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A9A59A-F5CF-4552-9F25-AAECB2F2B520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>Module Name</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Notes:</t>
-  </si>
-  <si>
-    <t>The GM internal name of the modual refrecenced</t>
   </si>
   <si>
     <t>The ID of this modual in decimal format. Max = 64 (6 bits)</t>
@@ -430,6 +427,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -438,36 +465,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,7 +749,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,15 +770,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -789,7 +786,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -797,7 +794,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -805,7 +802,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -813,7 +810,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -821,7 +818,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -838,7 +835,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,16 +849,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="91.35" customHeight="1" x14ac:dyDescent="0.3">
@@ -869,30 +866,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -900,16 +897,16 @@
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -917,13 +914,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -931,13 +928,13 @@
     </row>
     <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -963,10 +960,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
@@ -975,12 +972,12 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -988,7 +985,7 @@
     </row>
     <row r="4" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -996,7 +993,7 @@
     </row>
     <row r="5" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1013,7 +1010,7 @@
   <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1109,44 +1106,44 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1270,7 +1267,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1278,7 +1275,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1286,10 +1283,10 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1306,17 +1303,17 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1334,319 +1331,319 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="17">
+        <v>13</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="20">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="20">
-        <v>13</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="22" t="s">
+      <c r="J3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="K3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="L3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="M3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="N3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="O3" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="P3" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="P3" s="22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>69</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" t="s">
         <v>70</v>
       </c>
-      <c r="D6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>71</v>
       </c>
-      <c r="J6" t="s">
-        <v>72</v>
-      </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
       <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
         <v>68</v>
       </c>
-      <c r="E10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" t="s">
-        <v>69</v>
-      </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="B14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
       <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
         <v>68</v>
       </c>
-      <c r="E14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" t="s">
-        <v>69</v>
-      </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" t="s">
         <v>79</v>
-      </c>
-      <c r="J15" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[feat] lots of work to rx messages
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calja\GitHub Files\Gopher Motorsports\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A9A59A-F5CF-4552-9F25-AAECB2F2B520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A354EC-0E83-492D-9EA7-C6258D3472F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="3" r:id="rId2"/>
     <sheet name="Commands" sheetId="4" r:id="rId3"/>
-    <sheet name="ID Example" sheetId="2" r:id="rId4"/>
-    <sheet name="Full Message Examples" sheetId="5" r:id="rId5"/>
+    <sheet name="Errors" sheetId="6" r:id="rId4"/>
+    <sheet name="ID Example" sheetId="2" r:id="rId5"/>
+    <sheet name="Full Message Examples" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
   <si>
     <t>Module Name</t>
   </si>
@@ -272,6 +273,24 @@
   </si>
   <si>
     <t>0x1</t>
+  </si>
+  <si>
+    <t>Note: Parameter Data is sent in big endian</t>
+  </si>
+  <si>
+    <t>CAN Error Example</t>
+  </si>
+  <si>
+    <t>PARAM_NOT_FOUND</t>
+  </si>
+  <si>
+    <t>ID_NOT_FOUND</t>
+  </si>
+  <si>
+    <t>PARAM_NOT_ENABLED</t>
+  </si>
+  <si>
+    <t>SIZE_ERROR</t>
   </si>
 </sst>
 </file>
@@ -835,7 +854,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,7 +969,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,6 +1025,65 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD9C4D-9A56-475A-A0E0-AB31F55D4DB1}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
@@ -1326,12 +1404,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8270471-FF49-4B7E-9E01-25107B918C4F}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1440,6 +1518,9 @@
       <c r="A5" s="8" t="s">
         <v>44</v>
       </c>
+      <c r="I5" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1461,10 +1542,10 @@
         <v>68</v>
       </c>
       <c r="I6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" t="s">
         <v>70</v>
-      </c>
-      <c r="J6" t="s">
-        <v>71</v>
       </c>
       <c r="K6" t="s">
         <v>66</v>
@@ -1646,7 +1727,77 @@
         <v>79</v>
       </c>
     </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" t="s">
+        <v>66</v>
+      </c>
+      <c r="O18" t="s">
+        <v>66</v>
+      </c>
+      <c r="P18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved error handling during RX
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calja\GitHub Files\Gopher Motorsports\STM32_CAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A354EC-0E83-492D-9EA7-C6258D3472F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B151DA3E-C59A-4A03-B3C1-8FC0EAAC2855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="91">
   <si>
     <t>Module Name</t>
   </si>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t>SIZE_ERROR</t>
+  </si>
+  <si>
+    <t>DATATYPE_NOT_FOUND</t>
+  </si>
+  <si>
+    <t>COMMAND_ID_NOT_FOUND</t>
+  </si>
+  <si>
+    <t>These will mostly be used during debugging, they should not reguarily populate the CAN bus</t>
+  </si>
+  <si>
+    <t>COMMAND_NOT_ENABLED</t>
   </si>
 </sst>
 </file>
@@ -771,12 +783,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
@@ -784,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="102" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -795,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -803,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -811,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -819,7 +831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -827,7 +839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -835,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -857,16 +869,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.07421875" customWidth="1"/>
+    <col min="2" max="2" width="25.765625" customWidth="1"/>
+    <col min="3" max="3" width="19.84375" customWidth="1"/>
+    <col min="4" max="4" width="14.69140625" customWidth="1"/>
+    <col min="5" max="5" width="23.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
         <v>18</v>
       </c>
@@ -880,7 +892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="91.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="91.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -897,7 +909,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -914,7 +926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -931,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -945,7 +957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -969,15 +981,15 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
         <v>28</v>
       </c>
@@ -985,7 +997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="37.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -1018,7 +1030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1026,18 +1038,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD9C4D-9A56-475A-A0E0-AB31F55D4DB1}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
         <v>28</v>
       </c>
@@ -1045,16 +1057,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>84</v>
       </c>
@@ -1062,20 +1076,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1091,9 +1129,9 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -1182,7 +1220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1223,7 +1261,7 @@
       <c r="AB2" s="22"/>
       <c r="AC2" s="22"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1254,7 +1292,7 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -1343,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -1384,7 +1422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="I10" s="11"/>
@@ -1409,12 +1447,12 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
@@ -1425,7 +1463,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="17">
         <v>0</v>
       </c>
@@ -1469,7 +1507,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1514,7 +1552,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>44</v>
       </c>
@@ -1522,7 +1560,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1566,7 +1604,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1586,12 +1624,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1635,7 +1673,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1655,12 +1693,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1704,7 +1742,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1727,12 +1765,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1776,7 +1814,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
No more TODOs - ready for code review!
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B151DA3E-C59A-4A03-B3C1-8FC0EAAC2855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF2BD4C-953D-4F83-BF34-796E9D1660D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
@@ -1040,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD9C4D-9A56-475A-A0E0-AB31F55D4DB1}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1125,11 +1125,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="29" width="7.61328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A1" s="3">

</xml_diff>

<commit_message>
Updated the example .c file and added lots of comments all over
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF2BD4C-953D-4F83-BF34-796E9D1660D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1FC3AE-41E9-4825-A94D-944F31B60B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="95">
   <si>
     <t>Module Name</t>
   </si>
@@ -125,9 +125,6 @@
     <t>INC_VARIABLE</t>
   </si>
   <si>
-    <t>TURN_FAN_OFF</t>
-  </si>
-  <si>
     <t>CUST_COMMAND_2</t>
   </si>
   <si>
@@ -303,6 +300,21 @@
   </si>
   <si>
     <t>COMMAND_NOT_ENABLED</t>
+  </si>
+  <si>
+    <t>SET_LED_STATE</t>
+  </si>
+  <si>
+    <t>REMOTE PARAMETER</t>
+  </si>
+  <si>
+    <t>a U8 of data that is sent with the command</t>
+  </si>
+  <si>
+    <t>UNUSED</t>
+  </si>
+  <si>
+    <t>the state to set the LED to</t>
   </si>
 </sst>
 </file>
@@ -911,7 +923,7 @@
     </row>
     <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -920,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -928,7 +940,7 @@
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
@@ -937,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -951,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -965,7 +977,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -978,61 +990,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB27F71-B657-4A76-B4D2-CB1DD8552EDE}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="23.69140625" customWidth="1"/>
+    <col min="4" max="4" width="17.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="37.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D1" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>30</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1062,15 +1091,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1078,7 +1107,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1086,7 +1115,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1094,7 +1123,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1102,7 +1131,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1110,7 +1139,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1125,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
@@ -1460,10 +1489,10 @@
         <v>29</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
@@ -1471,43 +1500,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>42</v>
       </c>
       <c r="D2" s="17">
         <v>13</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>61</v>
-      </c>
       <c r="N2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="P2" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
@@ -1527,89 +1556,89 @@
         <v>13</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
         <v>67</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" t="s">
         <v>69</v>
       </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" t="s">
-        <v>70</v>
-      </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1624,61 +1653,61 @@
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
         <v>67</v>
       </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
       <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" t="s">
-        <v>68</v>
-      </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -1690,7 +1719,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -1698,56 +1727,56 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
-      </c>
       <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" t="s">
         <v>67</v>
       </c>
-      <c r="E14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" t="s">
-        <v>68</v>
-      </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1759,67 +1788,67 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
         <v>78</v>
-      </c>
-      <c r="J15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
         <v>67</v>
       </c>
-      <c r="B18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1834,7 +1863,7 @@
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed lots of bugs and configuration errors, now appears to work as inteneded (but not extensivly tested)
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1FC3AE-41E9-4825-A94D-944F31B60B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF44BEB-B135-4EF2-9282-5D3611D15026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9617" yWindow="3814" windowWidth="24694" windowHeight="13157" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Request Value</t>
   </si>
   <si>
-    <t>Custom Command</t>
-  </si>
-  <si>
     <t>FAN_CURRENT</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>the state to set the LED to</t>
+  </si>
+  <si>
+    <t>Can Command</t>
   </si>
 </sst>
 </file>
@@ -792,7 +792,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -877,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -923,7 +923,7 @@
     </row>
     <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -940,16 +940,16 @@
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -963,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -971,13 +971,13 @@
     </row>
     <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB27F71-B657-4A76-B4D2-CB1DD8552EDE}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1004,13 +1004,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
@@ -1019,43 +1019,43 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1070,7 +1070,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1080,10 +1080,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
@@ -1091,15 +1091,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1486,13 +1486,13 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
@@ -1500,43 +1500,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>41</v>
       </c>
       <c r="D2" s="17">
         <v>13</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>60</v>
-      </c>
       <c r="N2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="P2" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
@@ -1556,89 +1556,89 @@
         <v>13</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" t="s">
-        <v>69</v>
-      </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1653,61 +1653,61 @@
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
         <v>66</v>
       </c>
-      <c r="B10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
       <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" t="s">
         <v>66</v>
       </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" t="s">
-        <v>67</v>
-      </c>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -1719,7 +1719,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -1727,56 +1727,56 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
       <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" t="s">
         <v>66</v>
       </c>
-      <c r="E14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" t="s">
-        <v>67</v>
-      </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1788,67 +1788,67 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" t="s">
         <v>77</v>
-      </c>
-      <c r="J15" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1863,7 +1863,7 @@
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for every parameter type, updated example
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF44BEB-B135-4EF2-9282-5D3611D15026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B28FF0-A693-47E9-9338-DE47DD7767E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9617" yWindow="3814" windowWidth="24694" windowHeight="13157" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="111">
   <si>
     <t>Module Name</t>
   </si>
@@ -315,6 +315,54 @@
   </si>
   <si>
     <t>Can Command</t>
+  </si>
+  <si>
+    <t>U8_TESTER</t>
+  </si>
+  <si>
+    <t>U16_TESTER</t>
+  </si>
+  <si>
+    <t>U32</t>
+  </si>
+  <si>
+    <t>U64</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S32</t>
+  </si>
+  <si>
+    <t>S64</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>U32_TESTER</t>
+  </si>
+  <si>
+    <t>S8_TESTER</t>
+  </si>
+  <si>
+    <t>S16_TESTER</t>
+  </si>
+  <si>
+    <t>S32_TESTER</t>
+  </si>
+  <si>
+    <t>S64_TESTER</t>
+  </si>
+  <si>
+    <t>FLOAT_TESTER</t>
+  </si>
+  <si>
+    <t>U64_TESTER</t>
   </si>
 </sst>
 </file>
@@ -875,10 +923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -980,8 +1028,137 @@
         <v>37</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8">
         <v>2</v>
       </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="2">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CAN requests now use the RTR bit of the can message. UNTESTED
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C31BC7-7087-4D20-A65D-BBC0A6B9BF51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE76C6F4-74CD-491B-8119-F7879ECA4D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="110">
   <si>
     <t>Module Name</t>
   </si>
@@ -107,9 +107,6 @@
     <t>The number of bytes this message needs for this parameter. This is directly related to the data type</t>
   </si>
   <si>
-    <t>Request Value</t>
-  </si>
-  <si>
     <t>FAN_CURRENT</t>
   </si>
   <si>
@@ -128,18 +125,12 @@
     <t>8 bits for command ID, 8 bits for function parameter</t>
   </si>
   <si>
-    <t>This will be used for requesting data from another module</t>
-  </si>
-  <si>
     <t>Max 255 (U8)</t>
   </si>
   <si>
     <t>COMMAND</t>
   </si>
   <si>
-    <t>REQ_PARAM</t>
-  </si>
-  <si>
     <t>U16</t>
   </si>
   <si>
@@ -245,12 +236,6 @@
     <t>Value = 1000</t>
   </si>
   <si>
-    <t>Req_Param</t>
-  </si>
-  <si>
-    <t>0x02</t>
-  </si>
-  <si>
     <t>CAN Command Example</t>
   </si>
   <si>
@@ -363,13 +348,25 @@
   </si>
   <si>
     <t>U64_TESTER</t>
+  </si>
+  <si>
+    <t>RTR bit</t>
+  </si>
+  <si>
+    <t>Requesting</t>
+  </si>
+  <si>
+    <t>Data Message</t>
+  </si>
+  <si>
+    <t>RTR Bit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,8 +395,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +481,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -491,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -548,6 +557,9 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -556,6 +568,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,10 +938,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25EEE5-CB71-4AB5-A058-2384CE79396F}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -969,63 +984,60 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1033,132 +1045,118 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="2">
+        <v>99</v>
+      </c>
+      <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="2">
+        <v>102</v>
+      </c>
+      <c r="C12">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C14">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="C16" s="2"/>
+      <c r="C15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1181,13 +1179,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
@@ -1196,43 +1194,43 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1257,10 +1255,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
@@ -1268,15 +1266,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1284,7 +1282,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1292,7 +1290,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1300,7 +1298,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1308,7 +1306,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1316,7 +1314,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1329,18 +1327,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76182EF-68F7-4F83-AD1B-7A6AB8CEA752}">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F17:AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="29" width="7.61328125" customWidth="1"/>
+    <col min="31" max="31" width="11.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -1428,49 +1427,55 @@
       <c r="AC1" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="AE1" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
       <c r="N2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AE2" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1501,7 +1506,7 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -1584,13 +1589,16 @@
         <v>0</v>
       </c>
       <c r="AB4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
         <v>1</v>
       </c>
-      <c r="AC4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="AE4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -1630,8 +1638,11 @@
       <c r="AC5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AE5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="I10" s="11"/>
@@ -1653,70 +1664,73 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8270471-FF49-4B7E-9E01-25107B918C4F}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="17">
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="17">
         <v>13</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="17" t="s">
+      <c r="O2" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="P2" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q2" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1732,90 +1746,96 @@
       <c r="E3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="19" t="s">
+      <c r="F3" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" t="s">
-        <v>64</v>
-      </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1829,62 +1849,68 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="F7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
       </c>
       <c r="J10" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -1896,64 +1922,67 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" t="s">
-        <v>75</v>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" t="s">
+        <v>63</v>
       </c>
       <c r="J14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1965,67 +1994,73 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>76</v>
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>108</v>
       </c>
       <c r="J15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
       </c>
       <c r="J18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -2039,8 +2074,11 @@
       <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="I19" t="s">
-        <v>81</v>
+      <c r="F19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RTR requesting is tested and working
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE76C6F4-74CD-491B-8119-F7879ECA4D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397E49B3-8743-4276-AE57-59E1320A0B12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="111">
   <si>
     <t>Module Name</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>RTR Bit</t>
+  </si>
+  <si>
+    <t>Requesting Data</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1670,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1925,7 +1928,7 @@
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
F7 is working like the F0
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397E49B3-8743-4276-AE57-59E1320A0B12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252995C5-C7A9-4EB1-914B-676550FC39F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moduals" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="112">
   <si>
     <t>Module Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>ACM</t>
   </si>
   <si>
-    <t>Display</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -363,6 +360,12 @@
   </si>
   <si>
     <t>Requesting Data</t>
+  </si>
+  <si>
+    <t>ALL_MODULES</t>
+  </si>
+  <si>
+    <t>DISPLAY</t>
   </si>
 </sst>
 </file>
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -879,23 +882,24 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -903,15 +907,15 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -919,18 +923,26 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -958,16 +970,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="91.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -975,30 +987,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1006,13 +1018,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1020,13 +1032,13 @@
     </row>
     <row r="5" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1034,13 +1046,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1048,13 +1060,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1062,13 +1074,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -1076,13 +1088,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1090,13 +1102,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1104,13 +1116,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1118,13 +1130,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1132,13 +1144,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13">
         <v>8</v>
@@ -1146,13 +1158,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1182,13 +1194,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
@@ -1197,43 +1209,43 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1258,10 +1270,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
@@ -1269,15 +1281,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1285,7 +1297,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1293,7 +1305,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1301,7 +1313,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1309,7 +1321,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1317,7 +1329,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1431,15 +1443,15 @@
         <v>28</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
@@ -1447,7 +1459,7 @@
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
@@ -1455,10 +1467,10 @@
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
@@ -1475,7 +1487,7 @@
       <c r="AB2" s="23"/>
       <c r="AC2" s="23"/>
       <c r="AE2" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.4">
@@ -1603,7 +1615,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1622,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1639,10 +1651,10 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AE5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -1669,21 +1681,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8270471-FF49-4B7E-9E01-25107B918C4F}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
@@ -1691,154 +1703,154 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="D2" s="17">
         <v>13</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>56</v>
-      </c>
       <c r="O2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" t="s">
-        <v>65</v>
-      </c>
       <c r="L6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1847,73 +1859,73 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
         <v>62</v>
       </c>
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
       <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -1922,70 +1934,70 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
-      </c>
       <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
         <v>62</v>
       </c>
-      <c r="E14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" t="s">
-        <v>63</v>
-      </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1994,76 +2006,76 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" t="s">
         <v>71</v>
-      </c>
-      <c r="K15" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -2072,16 +2084,16 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pre-processor options for multiple CAN busses. UNTESTED
</commit_message>
<xml_diff>
--- a/GopherCAN.xlsx
+++ b/GopherCAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_files\STM32_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252995C5-C7A9-4EB1-914B-676550FC39F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBDB152-AE5D-44DD-B55B-08AAD7FA68A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="119">
   <si>
     <t>Module Name</t>
   </si>
@@ -44,9 +44,6 @@
     <t>The ID of this modual in decimal format. Max = 64 (6 bits)</t>
   </si>
   <si>
-    <t>ECM</t>
-  </si>
-  <si>
     <t>EDL</t>
   </si>
   <si>
@@ -366,13 +363,37 @@
   </si>
   <si>
     <t>DISPLAY</t>
+  </si>
+  <si>
+    <t>Which bus this module is on</t>
+  </si>
+  <si>
+    <t>DLM</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t>Bus Id</t>
+  </si>
+  <si>
+    <t>ALL_BUSSES</t>
+  </si>
+  <si>
+    <t>GCAN0</t>
+  </si>
+  <si>
+    <t>GCAN1</t>
+  </si>
+  <si>
+    <t>GCAN2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +427,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -566,6 +593,9 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -574,9 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -869,83 +896,111 @@
     <col min="2" max="2" width="15.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="102" x14ac:dyDescent="0.4">
+      <c r="D1" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="102" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D2" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="2">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -970,16 +1025,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="91.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -987,30 +1042,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1018,13 +1073,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1032,13 +1087,13 @@
     </row>
     <row r="5" spans="1:5" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1046,13 +1101,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1060,13 +1115,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1074,13 +1129,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -1088,13 +1143,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1102,13 +1157,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1116,13 +1171,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1130,13 +1185,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1144,13 +1199,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13">
         <v>8</v>
@@ -1158,13 +1213,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1194,13 +1249,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
@@ -1209,43 +1264,43 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1270,10 +1325,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
@@ -1281,15 +1336,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1297,7 +1352,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1305,7 +1360,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1313,7 +1368,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1321,7 +1376,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1329,7 +1384,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1443,51 +1498,51 @@
         <v>28</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
       <c r="AE2" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.4">
@@ -1615,7 +1670,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1623,7 +1678,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1631,10 +1686,10 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1651,10 +1706,10 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AE5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -1689,13 +1744,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
@@ -1703,397 +1758,397 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>36</v>
       </c>
       <c r="D2" s="17">
         <v>13</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="O2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>56</v>
+        <v>105</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>49</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" t="s">
-        <v>64</v>
-      </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
       <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
         <v>61</v>
       </c>
-      <c r="E10" t="s">
-        <v>62</v>
-      </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
       <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" t="s">
-        <v>62</v>
-      </c>
       <c r="J14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
         <v>70</v>
-      </c>
-      <c r="K15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
-      </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>